<commit_message>
Another Commit from Me
</commit_message>
<xml_diff>
--- a/src/test/resources/excelsheets/testdata.xlsx
+++ b/src/test/resources/excelsheets/testdata.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himun\eclipse-workspace\phase1\src\test\resources\excelsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2FA74F-B9BD-49F7-88A9-B5AEBED4CB26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9252DB0-5F77-47F1-BBC5-9ACD1B28020F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="addCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="openAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="deleteCustomers" sheetId="4" r:id="rId2"/>
+    <sheet name="addCustomerTest" sheetId="1" r:id="rId3"/>
+    <sheet name="openAccountTest" sheetId="2" r:id="rId4"/>
+    <sheet name="customerLogin" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -78,6 +80,9 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -397,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1356C15-851B-447E-A1B5-4263DC38DFA0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -435,6 +440,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{411BAA78-E1F8-4ED5-8AFE-DF62972AC2AE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -477,7 +507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E70E5-B823-49AC-8DC4-2F08E9A41FE1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -515,4 +545,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E13C55-DA26-498C-90FB-DFE2457F19DC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>